<commit_message>
add conditional context menu
</commit_message>
<xml_diff>
--- a/icons.xlsx
+++ b/icons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\Projets\WindowsScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4223F7-23C0-4BD6-9C2F-89006F226809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC549140-835D-4B2A-9911-EFFB6E66A217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <r>
       <t>"Icon"="</t>
@@ -38,6 +38,29 @@
         <family val="3"/>
       </rPr>
       <t>%windir%\\System32\\shell32.dll,262</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"Icon"="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%systemroot%\\system32\\imageres.dll,18</t>
     </r>
     <r>
       <rPr>
@@ -243,6 +266,707 @@
         <a:xfrm>
           <a:off x="638175" y="1524000"/>
           <a:ext cx="200025" cy="568071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>185573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F569B9E-D226-4C32-97D8-ACAA275A5C24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="2095500"/>
+          <a:ext cx="238125" cy="566573"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22188</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>6315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219017</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4794</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D965726E-B2B7-4E41-98A1-93F213D2D713}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="10713" t="51013"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4280423" y="582618"/>
+          <a:ext cx="196829" cy="190579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>16009</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4001</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200105</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28490AA6-80FE-4083-BB2D-B34FD059CDFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="15159" t="8459" r="3584" b="44906"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4274244" y="388203"/>
+          <a:ext cx="184096" cy="187390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238628</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{076DCCD7-1195-4F95-8C01-7600E30C64B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="-3927" t="11094"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6105526" y="561976"/>
+          <a:ext cx="229102" cy="342972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>202510</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C43CD923-1593-472C-B748-86729E3224C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="2676526"/>
+          <a:ext cx="173935" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>27710</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>35502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200892</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>174048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{611E45B6-D11A-4321-90CC-AA7474EA754C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="637310" y="3274002"/>
+          <a:ext cx="173182" cy="519546"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9164</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>29540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209945</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>170571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52AD0069-81BB-4FAF-9B97-E17F17E477F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1837964" y="410540"/>
+          <a:ext cx="200781" cy="522031"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16445</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>21451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193132</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>188181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A354BFD-2CEA-4A95-90D6-68F5C6ABFA52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1845245" y="973951"/>
+          <a:ext cx="176687" cy="547730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8660</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>18188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>181866</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>947</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE28197D-4AEB-4099-85C4-3E169EF33CFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="846860" y="1542188"/>
+          <a:ext cx="173206" cy="554259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16887</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>27280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>164112</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC6B544-9392-45EC-9CA2-37030A064A4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="855087" y="2122780"/>
+          <a:ext cx="147225" cy="545599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7015</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>32908</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>164459</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176722</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F87F203B-1EEF-4FF5-99D7-E0294E0E1D03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="845215" y="2699908"/>
+          <a:ext cx="157444" cy="524814"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10647</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>170353</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>183296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95CBC37-CE5A-493D-ACBD-1309FE415D36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="848847" y="3264838"/>
+          <a:ext cx="159706" cy="537958"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10393</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9096</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>218240</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>515</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E70E20-4413-48CE-ABFD-5C695B1CBECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1724893" y="390096"/>
+          <a:ext cx="207847" cy="562919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10367</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180160</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436D64DE-BF05-49A5-9430-D3FFE1B6BCA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1724867" y="967660"/>
+          <a:ext cx="169793" cy="560318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9354</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>5502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219279</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>175557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230DA72D-F8A8-426F-BEF2-144A4C492038}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1361904" y="1529502"/>
+          <a:ext cx="209925" cy="551055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>17319</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>24163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>192257</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>185470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D977555B-F14F-42AE-8E7B-EB8BBF67DE09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1369869" y="2119663"/>
+          <a:ext cx="174938" cy="542307"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -517,62 +1241,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>280</v>
+      </c>
+      <c r="E3">
+        <v>298</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>263</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>281</v>
+      </c>
+      <c r="E4">
+        <v>299</v>
+      </c>
+      <c r="I4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>264</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>282</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>265</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>283</v>
+      </c>
+      <c r="E6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>266</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>284</v>
+      </c>
+      <c r="E7">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>267</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>285</v>
+      </c>
+      <c r="E8">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>268</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>286</v>
+      </c>
+      <c r="E9">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>269</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>287</v>
+      </c>
+      <c r="E10">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>270</v>
+      </c>
+      <c r="C11">
+        <v>288</v>
+      </c>
+      <c r="E11">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>271</v>
+      </c>
+      <c r="C12">
+        <v>289</v>
+      </c>
+      <c r="E12">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>272</v>
+      </c>
+      <c r="C13">
+        <v>290</v>
+      </c>
+      <c r="E13">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>273</v>
+      </c>
+      <c r="C14">
+        <v>291</v>
+      </c>
+      <c r="E14">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>274</v>
+      </c>
+      <c r="C15">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>275</v>
+      </c>
+      <c r="C16">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>276</v>
+      </c>
+      <c r="C17">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>277</v>
+      </c>
+      <c r="C18">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>278</v>
+      </c>
+      <c r="C19">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>279</v>
+      </c>
+      <c r="C20">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>